<commit_message>
first version of the entire report
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZLaP\Desktop\PFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6527AB-B25F-40BA-B2E9-8DEBB26A06C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6A9C69-60C5-464A-9A73-07DC1D24241F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="164">
   <si>
     <t>GANTT CHART TEMPLATE</t>
   </si>
@@ -248,145 +248,292 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t xml:space="preserve"> Spécifications générales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Identification des besoins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Spécifications  fonctionnelles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Comprendre le fonctionnement  de service scaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Comprendre le fonctionnement  de service watcher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Comprendre l'architecture Microservice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Formation C#,Solid,UnitTesting …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Les tests d'intégration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   les tests unitaires  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   les tests d'integration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">START DATE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">END DATE </t>
+  </si>
+  <si>
+    <t>WORK DAYS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Les tests unitaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Intégrer IConfigurationHlder à la solution existante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Documentation sur l'objet de configuration Json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Extraire une unité de configuration à partir d'un fichier Json  </t>
+  </si>
+  <si>
+    <t>10jours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                GANTT Diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Spécifications Techniques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Conception des interfaces : Configuration, ClientRequest, et Worker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Implémentation des interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Analyse des événements de la queue (enqueue, dequeue,...)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Conception de l'objet simulateur (StartSimulation,EndSimulation)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Analyse des fonctionnalités de base de service de scaling (ScaleUp,ScaleDown, GetNextScalingDate ...)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">   Gérer les dépendances du temps entre les différentes interfaces (Injecter la dépendance du temps)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Les tests unitaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Conception de l'interface MetricCloud (getIdleTime,GetCost...)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Conception de l'objet Orchestrator (GetNextEvent...)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Générer le fichier de résultas des workers : workers_result.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Générer un fichier de résultas des requestes : requests_Result.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Implémentation de l'interface MetricCloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Génération de fichier pour les metrics Cloud : metrics.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Les tests d'intégration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Benchmarking Métriques cloud les plus expressives</t>
+  </si>
+  <si>
+    <t>14/2/2020</t>
+  </si>
+  <si>
+    <t>5jours</t>
+  </si>
+  <si>
+    <t>15/5/2020</t>
+  </si>
+  <si>
+    <t>18/5/2020</t>
+  </si>
+  <si>
+    <t>22/5/2020</t>
+  </si>
+  <si>
+    <t>25/5/2020</t>
+  </si>
+  <si>
+    <t>29/5/2020</t>
+  </si>
+  <si>
+    <t>Tests de validation</t>
+  </si>
+  <si>
+    <t>15/6/2020</t>
+  </si>
+  <si>
+    <t>19/6/2020</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Manuel d'utilisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Manuel de référence</t>
+  </si>
+  <si>
+    <t>22/6/2020</t>
+  </si>
+  <si>
+    <t>26/6/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Test de validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Retour d'expérience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Documentation sur le fonctionnement d'un worker cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Extraction des requêtes clients à partir d'un fichier csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Itération 1 : Récupération des données &amp; implémentation des objets de base</t>
+  </si>
+  <si>
+    <t>10 jours</t>
+  </si>
+  <si>
+    <t>21/2/2020</t>
+  </si>
+  <si>
+    <t>17/2/2020</t>
+  </si>
+  <si>
+    <t>20/2/2020</t>
+  </si>
+  <si>
+    <t>4jours</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Itération 2 : Implémentation du simulaterQueue &amp; simulaterWorkers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Analyse des fonctionnalités  de CloudWorkers (addWorker, shutDownWorker, AffectRequest…)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Conception de l'interface SimulaterQueue &amp; SimulaterWorkers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Implémenter l'interface SimulaterCloud &amp; SimulaterWorkers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Conception de l'interface SilulationResultPrinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Implémenatation de SimulationResultPrinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Afficher les de la simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Itération 3 : Implémenter le ScalerSimulater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Conception de l'objet ScalerSimulater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Implémenter l'interface ScalerSimulater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Implémenter l'objet DateTimeSimulater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Extension de l'objet configuration pour  couvrir les jours de la semaine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Implémenter  l'interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Conception de l'interface IConfigurationHolder qui représente une configuration hebdomadaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Itération 4 : Implémenter Simulator &amp; Orchestrator &amp; Commencer les tests d'intégration</t>
+  </si>
+  <si>
+    <t>Itération 7 : Implémenter les Métriques</t>
+  </si>
+  <si>
+    <t>Itération 6 :Implémentation du Simulation ResultPrinter</t>
+  </si>
+  <si>
     <t>7jours</t>
   </si>
   <si>
-    <t>3jours</t>
-  </si>
-  <si>
-    <t>4jours</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Spécifications générales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Identification des besoins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Spécifications  fonctionnelles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Spécifications non fonctionnelles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Comprendre le fonctionnement  de service scaling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Comprendre le fonctionnement  de service watcher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Comprendre l'architecture Microservice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Formation C#,Solid,UnitTesting …</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Implémenter les interfaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Les tests d'intégration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Gérer les dépendances du temps entre les différentes interfaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Itération 3 : Refactoring du code &amp; Adaptation aux normes SOLID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Implémentetr l'interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   les tests unitaires  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   les tests d'integration </t>
-  </si>
-  <si>
-    <t xml:space="preserve">START DATE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">END DATE </t>
-  </si>
-  <si>
-    <t>WORK DAYS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Les tests unitaires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Générer le fichier des résults des workers</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Itération 4 : Afficher l'état des workers et Implémenter les testes d'intégration</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Itération 5 : Extendre la configuration et Afficher le temps d'exécution des requetes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Intégrer IConfigurationHlder à la solution existante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Générer un fichier qui contient le temps d'exécution et le temps d'attente de chaque requete </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Itération 1 : Implémentation des fonctionnalités de base</t>
-  </si>
-  <si>
-    <t>8jours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Création de l'interface IConfigurationHolder qui représente une configuration hebdomadaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Documentation sur l'objet de configuration Json</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Extraction des  requetes clients à partir d'un fichier csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Extraire une unité de configuration à partir d'un fichier Json  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Conception de la structure de donnée  pour le simulateiur Cloud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Conception de la notion du temps de simulateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Implémenter les fonctionnalités du temps (GetTime,SetTime,addSeconds...)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Extension de l'objet configuartion pour  couvrir les jours de la semaine</t>
-  </si>
-  <si>
-    <t>10 jours</t>
-  </si>
-  <si>
-    <t>10jours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Conception des  des interfaces Configuration, ClientRequest, et Worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Décomposition de l'interface CloudSimulator en sous Interfaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Création des interfaces (QueueSimlator,ScalerSimulatro,Orchestrator)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Itération 2 : Implémentation du cloud Simulateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Implémenter les fonctionnaités de simulateur cloud (Queue,Scaler,LoadBalnacing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                                                GANTT Diagram</t>
-  </si>
-  <si>
-    <t>Itération 6 : Affichage des logs</t>
-  </si>
-  <si>
-    <t>Itération 7 : Implémenter les Métriques</t>
+    <t>20/3/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Documentation sur la tarification de Azure</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Itération 5 : Extendre l'objet de configuration : IConfigurationHolderHolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Générer un fichier de résultas des requestes : rmetrics_Result.csv</t>
+  </si>
+  <si>
+    <t>Warning : Suspension à cause de la pandémie Covid 19 (20/03 et 04/05)</t>
+  </si>
+  <si>
+    <t>25/6/2020</t>
+  </si>
+  <si>
+    <t>Itération 6 : Implémenter les Métriques</t>
+  </si>
+  <si>
+    <t>Itération 7 :Implémentation du Simulation ResultPrinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Conception de l'interface SimulationResultPrinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Afficher les résultats de la simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Implémentation de SimulationResultPrinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Générer un fichier de résultats des requestes : rmetrics_Result.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Générer un fichier de résultats des requestes : requests_Result.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Générer le fichier de résultats des workers : workers_result.csv</t>
   </si>
 </sst>
 </file>
@@ -397,25 +544,11 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="m&quot;/&quot;d"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="36">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -527,23 +660,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF434343"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -551,50 +667,97 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF434343"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="17">
@@ -824,271 +987,351 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="11" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="13" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="11" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="13" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="29" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="30" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="30" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="16" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="16" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="30" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="23" fillId="16" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="35" fillId="16" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="31" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="27" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="2" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2293,80 +2536,80 @@
       <c r="AJ5" s="2"/>
     </row>
     <row r="6" spans="1:36" ht="14.4">
-      <c r="A6" s="110"/>
-      <c r="B6" s="110" t="s">
+      <c r="A6" s="147"/>
+      <c r="B6" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="147" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="110" t="s">
+      <c r="D6" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="110" t="s">
+      <c r="E6" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="110" t="s">
+      <c r="F6" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="110" t="s">
+      <c r="G6" s="147" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="110" t="s">
+      <c r="H6" s="147" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="110" t="s">
+      <c r="I6" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="110" t="s">
+      <c r="J6" s="147" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="113"/>
-      <c r="L6" s="111"/>
-      <c r="M6" s="111"/>
-      <c r="N6" s="111"/>
-      <c r="O6" s="111"/>
-      <c r="P6" s="113" t="s">
+      <c r="K6" s="150"/>
+      <c r="L6" s="148"/>
+      <c r="M6" s="148"/>
+      <c r="N6" s="148"/>
+      <c r="O6" s="148"/>
+      <c r="P6" s="150" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="111"/>
-      <c r="R6" s="111"/>
-      <c r="S6" s="111"/>
-      <c r="T6" s="111"/>
-      <c r="U6" s="112" t="s">
+      <c r="Q6" s="148"/>
+      <c r="R6" s="148"/>
+      <c r="S6" s="148"/>
+      <c r="T6" s="148"/>
+      <c r="U6" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="V6" s="111"/>
-      <c r="W6" s="111"/>
-      <c r="X6" s="111"/>
-      <c r="Y6" s="111"/>
-      <c r="Z6" s="113" t="s">
+      <c r="V6" s="148"/>
+      <c r="W6" s="148"/>
+      <c r="X6" s="148"/>
+      <c r="Y6" s="148"/>
+      <c r="Z6" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="AA6" s="111"/>
-      <c r="AB6" s="111"/>
-      <c r="AC6" s="111"/>
-      <c r="AD6" s="111"/>
-      <c r="AE6" s="112" t="s">
+      <c r="AA6" s="148"/>
+      <c r="AB6" s="148"/>
+      <c r="AC6" s="148"/>
+      <c r="AD6" s="148"/>
+      <c r="AE6" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="AF6" s="111"/>
-      <c r="AG6" s="111"/>
-      <c r="AH6" s="111"/>
-      <c r="AI6" s="111"/>
+      <c r="AF6" s="148"/>
+      <c r="AG6" s="148"/>
+      <c r="AH6" s="148"/>
+      <c r="AI6" s="148"/>
       <c r="AJ6" s="49"/>
     </row>
     <row r="7" spans="1:36" ht="14.4">
-      <c r="A7" s="111"/>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
+      <c r="A7" s="148"/>
+      <c r="B7" s="148"/>
+      <c r="C7" s="148"/>
+      <c r="D7" s="148"/>
+      <c r="E7" s="148"/>
+      <c r="F7" s="148"/>
+      <c r="G7" s="148"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
       <c r="K7" s="49"/>
       <c r="L7" s="49"/>
       <c r="M7" s="49"/>
@@ -3247,18 +3490,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AH57"/>
+  <dimension ref="A1:AH145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="113.44140625" customWidth="1"/>
-    <col min="2" max="2" width="105.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="155" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" style="121" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" style="121" customWidth="1"/>
     <col min="5" max="5" width="23.5546875" customWidth="1"/>
     <col min="6" max="6" width="29.5546875" customWidth="1"/>
     <col min="7" max="8" width="7.33203125" customWidth="1"/>
@@ -3271,8 +3514,8 @@
     <row r="1" spans="1:32" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="122"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="1"/>
@@ -3305,8 +3548,8 @@
     <row r="2" spans="1:32" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="122"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
@@ -3337,14 +3580,14 @@
       <c r="AF2" s="2"/>
     </row>
     <row r="3" spans="1:32" ht="30" customHeight="1">
-      <c r="A3" s="116" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
+      <c r="A3" s="154" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="155"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="155"/>
+      <c r="F3" s="155"/>
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -3372,12 +3615,12 @@
       <c r="AE3" s="5"/>
       <c r="AF3" s="5"/>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+    <row r="4" spans="1:32" ht="15.6" customHeight="1">
+      <c r="A4" s="95"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="96"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -3406,50 +3649,50 @@
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
     </row>
-    <row r="5" spans="1:32" ht="14.4">
-      <c r="A5" s="110"/>
-      <c r="B5" s="114" t="s">
+    <row r="5" spans="1:32" ht="30.6" customHeight="1">
+      <c r="A5" s="151"/>
+      <c r="B5" s="152" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="114" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="119" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="114" t="s">
-        <v>92</v>
-      </c>
-      <c r="F5" s="118"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="111"/>
-      <c r="N5" s="111"/>
-      <c r="O5" s="111"/>
-      <c r="P5" s="111"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="111"/>
-      <c r="S5" s="111"/>
-      <c r="T5" s="111"/>
-      <c r="U5" s="111"/>
-      <c r="V5" s="113"/>
-      <c r="W5" s="111"/>
-      <c r="X5" s="111"/>
-      <c r="Y5" s="111"/>
-      <c r="Z5" s="111"/>
-      <c r="AA5" s="112"/>
-      <c r="AB5" s="111"/>
-      <c r="AC5" s="111"/>
-      <c r="AD5" s="111"/>
-      <c r="AE5" s="111"/>
+      <c r="C5" s="152" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="158" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="157" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="156"/>
+      <c r="L5" s="150"/>
+      <c r="M5" s="148"/>
+      <c r="N5" s="148"/>
+      <c r="O5" s="148"/>
+      <c r="P5" s="148"/>
+      <c r="Q5" s="149"/>
+      <c r="R5" s="148"/>
+      <c r="S5" s="148"/>
+      <c r="T5" s="148"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="150"/>
+      <c r="W5" s="148"/>
+      <c r="X5" s="148"/>
+      <c r="Y5" s="148"/>
+      <c r="Z5" s="148"/>
+      <c r="AA5" s="149"/>
+      <c r="AB5" s="148"/>
+      <c r="AC5" s="148"/>
+      <c r="AD5" s="148"/>
+      <c r="AE5" s="148"/>
       <c r="AF5" s="49"/>
     </row>
     <row r="6" spans="1:32" ht="12.6" customHeight="1">
-      <c r="A6" s="111"/>
-      <c r="B6" s="115"/>
-      <c r="C6" s="115"/>
-      <c r="D6" s="120"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="118"/>
+      <c r="A6" s="151"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="159"/>
+      <c r="E6" s="153"/>
+      <c r="F6" s="156"/>
       <c r="G6" s="76"/>
       <c r="H6" s="76"/>
       <c r="I6" s="76"/>
@@ -3477,16 +3720,21 @@
       <c r="AE6" s="49"/>
       <c r="AF6" s="49"/>
     </row>
-    <row r="7" spans="1:32" ht="21">
-      <c r="B7" s="91" t="s">
+    <row r="7" spans="1:32" ht="23.4">
+      <c r="A7" s="93"/>
+      <c r="B7" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="98" t="s">
-        <v>109</v>
-      </c>
-      <c r="F7" s="88"/>
+      <c r="C7" s="99">
+        <v>43892</v>
+      </c>
+      <c r="D7" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="100" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="86"/>
       <c r="G7" s="77"/>
       <c r="H7" s="78"/>
       <c r="I7" s="79"/>
@@ -3514,23 +3762,23 @@
       <c r="AE7" s="54"/>
       <c r="AF7" s="54"/>
     </row>
-    <row r="8" spans="1:32" ht="10.199999999999999" customHeight="1">
-      <c r="B8" s="93"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="88"/>
-    </row>
-    <row r="9" spans="1:32" ht="16.8" customHeight="1">
+    <row r="8" spans="1:32" ht="15.6" customHeight="1">
+      <c r="A8" s="93"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="117"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="86"/>
+    </row>
+    <row r="9" spans="1:32" ht="23.4" customHeight="1">
+      <c r="A9" s="93"/>
       <c r="B9" s="94" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="102" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="88"/>
+        <v>75</v>
+      </c>
+      <c r="C9" s="102"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="86"/>
       <c r="G9" s="80"/>
       <c r="H9" s="80"/>
       <c r="I9" s="80"/>
@@ -3558,16 +3806,15 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
     </row>
-    <row r="10" spans="1:32" ht="17.399999999999999" customHeight="1">
+    <row r="10" spans="1:32" ht="25.2" customHeight="1">
+      <c r="A10" s="93"/>
       <c r="B10" s="94" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="100"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="102" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="88"/>
+        <v>76</v>
+      </c>
+      <c r="C10" s="102"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="86"/>
       <c r="G10" s="80"/>
       <c r="H10" s="80"/>
       <c r="I10" s="80"/>
@@ -3595,16 +3842,15 @@
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
     </row>
-    <row r="11" spans="1:32" ht="15.6" customHeight="1">
+    <row r="11" spans="1:32" ht="26.4" customHeight="1">
+      <c r="A11" s="93"/>
       <c r="B11" s="94" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="100"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="103" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" s="88"/>
+        <v>77</v>
+      </c>
+      <c r="C11" s="102"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="86"/>
       <c r="G11" s="80"/>
       <c r="H11" s="80"/>
       <c r="I11" s="80"/>
@@ -3632,492 +3878,1263 @@
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
     </row>
-    <row r="12" spans="1:32" ht="15" customHeight="1">
-      <c r="A12" t="s">
+    <row r="12" spans="1:32" ht="25.8" customHeight="1">
+      <c r="A12" s="93" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="94" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="100"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="103" t="s">
-        <v>110</v>
-      </c>
-      <c r="F12" s="88"/>
+        <v>78</v>
+      </c>
+      <c r="C12" s="102"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="86"/>
       <c r="G12" s="81"/>
       <c r="H12" s="81"/>
       <c r="I12" s="81"/>
       <c r="J12" s="81"/>
       <c r="K12" s="81"/>
     </row>
-    <row r="13" spans="1:32" ht="20.399999999999999">
-      <c r="A13" s="109" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="90" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="108" t="s">
+    <row r="13" spans="1:32" s="136" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A13" s="137"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
+    </row>
+    <row r="14" spans="1:32" ht="26.4" customHeight="1">
+      <c r="A14" s="106"/>
+      <c r="B14" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="88"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-    </row>
-    <row r="14" spans="1:32" ht="11.4" customHeight="1">
-      <c r="B14" s="93"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="88"/>
-    </row>
-    <row r="15" spans="1:32" ht="17.399999999999999" customHeight="1">
-      <c r="B15" s="94" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="100"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="103" t="s">
+      <c r="C14" s="99" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="99" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="107" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="86"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+    </row>
+    <row r="15" spans="1:32" ht="13.2" customHeight="1">
+      <c r="A15" s="93"/>
+      <c r="B15" s="101"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="117"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="86"/>
+    </row>
+    <row r="16" spans="1:32" ht="26.4" customHeight="1">
+      <c r="A16" s="93"/>
+      <c r="B16" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="88"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-    </row>
-    <row r="16" spans="1:32" ht="15.6" customHeight="1">
-      <c r="B16" s="94" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="100"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="103" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="88"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="86"/>
       <c r="G16" s="81"/>
       <c r="H16" s="81"/>
       <c r="I16" s="81"/>
       <c r="J16" s="81"/>
       <c r="K16" s="81"/>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1">
+    <row r="17" spans="1:11" ht="24.6" customHeight="1">
+      <c r="A17" s="93"/>
       <c r="B17" s="94" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="100"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="103" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="88"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="86"/>
       <c r="G17" s="81"/>
       <c r="H17" s="81"/>
       <c r="I17" s="81"/>
       <c r="J17" s="81"/>
       <c r="K17" s="81"/>
     </row>
-    <row r="18" spans="1:11" ht="20.399999999999999">
-      <c r="A18" s="109" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="91" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="97"/>
-      <c r="D18" s="97"/>
-      <c r="E18" s="130" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="88"/>
+    <row r="18" spans="1:11" ht="25.8" customHeight="1">
+      <c r="A18" s="93"/>
+      <c r="B18" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="102"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="86"/>
       <c r="G18" s="81"/>
       <c r="H18" s="81"/>
       <c r="I18" s="81"/>
       <c r="J18" s="81"/>
       <c r="K18" s="81"/>
     </row>
-    <row r="19" spans="1:11" s="72" customFormat="1" ht="13.8" customHeight="1">
-      <c r="A19" s="109"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="99"/>
-      <c r="D19" s="99"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-    </row>
-    <row r="20" spans="1:11" s="105" customFormat="1" ht="13.8" customHeight="1">
-      <c r="A20" s="109"/>
-      <c r="B20" s="93" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
-      <c r="K20" s="83"/>
-    </row>
-    <row r="21" spans="1:11" ht="16.2" customHeight="1">
-      <c r="B21" s="94" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="100"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="88"/>
+    <row r="19" spans="1:11" s="136" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A19" s="137"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="105"/>
+      <c r="F19" s="138"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="83"/>
+      <c r="J19" s="83"/>
+      <c r="K19" s="83"/>
+    </row>
+    <row r="20" spans="1:11" ht="26.4" customHeight="1">
+      <c r="A20" s="106"/>
+      <c r="B20" s="98" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="99" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="99">
+        <v>43864</v>
+      </c>
+      <c r="E20" s="107" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" s="86"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+    </row>
+    <row r="21" spans="1:11" s="72" customFormat="1" ht="13.8" customHeight="1">
+      <c r="A21" s="106"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="86"/>
       <c r="G21" s="81"/>
       <c r="H21" s="81"/>
       <c r="I21" s="81"/>
       <c r="J21" s="81"/>
       <c r="K21" s="81"/>
     </row>
-    <row r="22" spans="1:11" ht="15.6" customHeight="1">
-      <c r="B22" s="94" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="100"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-    </row>
-    <row r="23" spans="1:11" s="82" customFormat="1" ht="15.6" customHeight="1">
-      <c r="B23" s="94" t="s">
-        <v>111</v>
-      </c>
-      <c r="C23" s="100"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="88"/>
+    <row r="22" spans="1:11" s="91" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A22" s="106"/>
+      <c r="B22" s="101" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="83"/>
+      <c r="K22" s="83"/>
+    </row>
+    <row r="23" spans="1:11" s="88" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A23" s="106"/>
+      <c r="B23" s="101" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="86"/>
       <c r="G23" s="83"/>
       <c r="H23" s="83"/>
       <c r="I23" s="83"/>
       <c r="J23" s="83"/>
       <c r="K23" s="83"/>
     </row>
-    <row r="24" spans="1:11" s="82" customFormat="1" ht="16.2" customHeight="1">
+    <row r="24" spans="1:11" ht="24" customHeight="1">
+      <c r="A24" s="93"/>
       <c r="B24" s="94" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="100"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="83"/>
-      <c r="K24" s="83"/>
-    </row>
-    <row r="25" spans="1:11" s="72" customFormat="1" ht="15.6" customHeight="1">
+        <v>125</v>
+      </c>
+      <c r="C24" s="102"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="81"/>
+    </row>
+    <row r="25" spans="1:11" ht="25.2" customHeight="1">
+      <c r="A25" s="93"/>
       <c r="B25" s="94" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="100"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="103"/>
-      <c r="F25" s="88"/>
+        <v>88</v>
+      </c>
+      <c r="C25" s="102"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="105"/>
+      <c r="F25" s="86"/>
       <c r="G25" s="81"/>
       <c r="H25" s="81"/>
       <c r="I25" s="81"/>
       <c r="J25" s="81"/>
       <c r="K25" s="81"/>
     </row>
-    <row r="26" spans="1:11" ht="19.8" customHeight="1">
-      <c r="A26" s="2"/>
-      <c r="B26" s="91" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" s="98"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="98" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="88"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="81"/>
-      <c r="I26" s="81"/>
-      <c r="J26" s="81"/>
-      <c r="K26" s="81"/>
-    </row>
-    <row r="27" spans="1:11" ht="12.6" customHeight="1">
-      <c r="A27" s="2"/>
-      <c r="B27" s="92"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="81"/>
-      <c r="I27" s="81"/>
-      <c r="J27" s="81"/>
-      <c r="K27" s="81"/>
-    </row>
-    <row r="28" spans="1:11" s="84" customFormat="1" ht="14.4" customHeight="1">
-      <c r="A28" s="2"/>
-      <c r="B28" s="92" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="83"/>
-      <c r="J28" s="83"/>
-      <c r="K28" s="83"/>
-    </row>
-    <row r="29" spans="1:11" s="82" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A29" s="2"/>
-      <c r="B29" s="93" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="83"/>
-      <c r="H29" s="83"/>
-      <c r="I29" s="83"/>
-      <c r="J29" s="83"/>
-      <c r="K29" s="83"/>
-    </row>
-    <row r="30" spans="1:11" s="75" customFormat="1" ht="15" customHeight="1">
-      <c r="A30" s="2"/>
-      <c r="B30" s="94" t="s">
+    <row r="26" spans="1:11" s="82" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A26" s="93"/>
+      <c r="B26" s="94" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="102"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="105"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="83"/>
+      <c r="J26" s="83"/>
+      <c r="K26" s="83"/>
+    </row>
+    <row r="27" spans="1:11" s="82" customFormat="1" ht="24" customHeight="1">
+      <c r="A27" s="93"/>
+      <c r="B27" s="94" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="87"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="88"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="83"/>
+      <c r="H27" s="83"/>
+      <c r="I27" s="83"/>
+      <c r="J27" s="83"/>
+      <c r="K27" s="83"/>
+    </row>
+    <row r="28" spans="1:11" s="72" customFormat="1" ht="28.8" customHeight="1">
+      <c r="A28" s="93"/>
+      <c r="B28" s="128" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="102"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="105"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="81"/>
+    </row>
+    <row r="29" spans="1:11" ht="24" customHeight="1">
+      <c r="A29" s="108"/>
+      <c r="B29" s="98" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="99">
+        <v>43892</v>
+      </c>
+      <c r="D29" s="99">
+        <v>44138</v>
+      </c>
+      <c r="E29" s="100" t="s">
+        <v>149</v>
+      </c>
+      <c r="F29" s="86"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="81"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="81"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.6" customHeight="1">
+      <c r="A30" s="108"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="108"/>
+      <c r="F30" s="86"/>
       <c r="G30" s="81"/>
       <c r="H30" s="81"/>
       <c r="I30" s="81"/>
       <c r="J30" s="81"/>
       <c r="K30" s="81"/>
     </row>
-    <row r="31" spans="1:11" ht="15.6">
-      <c r="B31" s="95" t="s">
+    <row r="31" spans="1:11" s="89" customFormat="1" ht="23.4" customHeight="1">
+      <c r="A31" s="108"/>
+      <c r="B31" s="101" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="118"/>
+      <c r="D31" s="118"/>
+      <c r="E31" s="108"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="83"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="83"/>
+    </row>
+    <row r="32" spans="1:11" s="91" customFormat="1" ht="23.4" customHeight="1">
+      <c r="A32" s="108"/>
+      <c r="B32" s="101" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="118"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="108"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="83"/>
+      <c r="J32" s="83"/>
+      <c r="K32" s="83"/>
+    </row>
+    <row r="33" spans="1:34" s="84" customFormat="1" ht="25.2" customHeight="1">
+      <c r="A33" s="108"/>
+      <c r="B33" s="101" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="108"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="83"/>
+      <c r="J33" s="83"/>
+      <c r="K33" s="83"/>
+    </row>
+    <row r="34" spans="1:34" s="82" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A34" s="108"/>
+      <c r="B34" s="101" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="108"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="83"/>
+      <c r="J34" s="83"/>
+      <c r="K34" s="83"/>
+    </row>
+    <row r="35" spans="1:34" s="75" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A35" s="108"/>
+      <c r="B35" s="94" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="108"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="81"/>
+    </row>
+    <row r="36" spans="1:34" s="89" customFormat="1" ht="23.4" customHeight="1">
+      <c r="A36" s="108"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="108"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="83"/>
+      <c r="J36" s="83"/>
+      <c r="K36" s="83"/>
+    </row>
+    <row r="37" spans="1:34" ht="23.4">
+      <c r="A37" s="93"/>
+      <c r="B37" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="119">
+        <v>44168</v>
+      </c>
+      <c r="D37" s="119" t="s">
+        <v>150</v>
+      </c>
+      <c r="E37" s="107" t="s">
+        <v>149</v>
+      </c>
+      <c r="F37" s="86"/>
+    </row>
+    <row r="38" spans="1:34" s="89" customFormat="1" ht="22.8">
+      <c r="A38" s="93"/>
+      <c r="B38" s="93"/>
+      <c r="C38" s="116"/>
+      <c r="D38" s="116"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="90"/>
+    </row>
+    <row r="39" spans="1:34" s="90" customFormat="1" ht="23.4">
+      <c r="A39" s="106"/>
+      <c r="B39" s="93" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="116"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="106"/>
+    </row>
+    <row r="40" spans="1:34" ht="23.4">
+      <c r="A40" s="93"/>
+      <c r="B40" s="101" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="116"/>
+      <c r="D40" s="116"/>
+      <c r="E40" s="93"/>
+      <c r="F40" s="86"/>
+    </row>
+    <row r="41" spans="1:34" ht="25.8" customHeight="1">
+      <c r="A41" s="93"/>
+      <c r="B41" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="116"/>
+      <c r="D41" s="116"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="86"/>
+    </row>
+    <row r="42" spans="1:34" ht="24" customHeight="1">
+      <c r="A42" s="93"/>
+      <c r="B42" s="101" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="116"/>
+      <c r="D42" s="116"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="86"/>
+    </row>
+    <row r="43" spans="1:34" s="136" customFormat="1" ht="24" customHeight="1">
+      <c r="A43" s="137"/>
+      <c r="B43" s="101"/>
+      <c r="C43" s="139"/>
+      <c r="D43" s="139"/>
+      <c r="E43" s="137"/>
+      <c r="F43" s="138"/>
+    </row>
+    <row r="44" spans="1:34" s="89" customFormat="1" ht="37.200000000000003" customHeight="1">
+      <c r="A44" s="93"/>
+      <c r="B44" s="126" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" s="125"/>
+      <c r="D44" s="125"/>
+      <c r="E44" s="124"/>
+      <c r="F44" s="90"/>
+    </row>
+    <row r="45" spans="1:34" s="85" customFormat="1" ht="26.4" customHeight="1">
+      <c r="A45" s="106"/>
+      <c r="B45" s="110" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="119">
+        <v>43926</v>
+      </c>
+      <c r="D45" s="119" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="107" t="s">
+        <v>89</v>
+      </c>
+      <c r="F45" s="86"/>
+      <c r="G45" s="86"/>
+      <c r="H45" s="86"/>
+      <c r="I45" s="86"/>
+      <c r="J45" s="86"/>
+      <c r="K45" s="86"/>
+      <c r="L45" s="86"/>
+      <c r="M45" s="86"/>
+      <c r="N45" s="86"/>
+      <c r="O45" s="86"/>
+      <c r="P45" s="86"/>
+      <c r="Q45" s="86"/>
+      <c r="R45" s="86"/>
+      <c r="S45" s="86"/>
+      <c r="T45" s="86"/>
+      <c r="U45" s="86"/>
+      <c r="V45" s="86"/>
+      <c r="W45" s="86"/>
+      <c r="X45" s="86"/>
+      <c r="Y45" s="86"/>
+      <c r="Z45" s="86"/>
+      <c r="AA45" s="86"/>
+      <c r="AB45" s="86"/>
+      <c r="AC45" s="86"/>
+      <c r="AD45" s="86"/>
+      <c r="AE45" s="86"/>
+      <c r="AF45" s="86"/>
+      <c r="AG45" s="86"/>
+      <c r="AH45" s="86"/>
+    </row>
+    <row r="46" spans="1:34" ht="15.6" customHeight="1">
+      <c r="A46" s="93"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="116"/>
+      <c r="D46" s="116"/>
+      <c r="E46" s="93"/>
+      <c r="F46" s="86"/>
+    </row>
+    <row r="47" spans="1:34" s="89" customFormat="1" ht="23.4">
+      <c r="A47" s="93"/>
+      <c r="B47" s="101" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="116"/>
+      <c r="D47" s="116"/>
+      <c r="E47" s="93"/>
+      <c r="F47" s="90"/>
+    </row>
+    <row r="48" spans="1:34" ht="26.4" customHeight="1">
+      <c r="A48" s="93"/>
+      <c r="B48" s="101" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="116"/>
+      <c r="D48" s="116"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="86"/>
+    </row>
+    <row r="49" spans="1:6" ht="25.8" customHeight="1">
+      <c r="A49" s="93"/>
+      <c r="B49" s="101" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="116"/>
+      <c r="D49" s="116"/>
+      <c r="E49" s="93"/>
+      <c r="F49" s="86"/>
+    </row>
+    <row r="50" spans="1:6" ht="24.6" customHeight="1">
+      <c r="A50" s="93"/>
+      <c r="B50" s="101" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="116"/>
+      <c r="D50" s="116"/>
+      <c r="E50" s="93"/>
+      <c r="F50" s="86"/>
+    </row>
+    <row r="51" spans="1:6" ht="24" customHeight="1">
+      <c r="A51" s="93"/>
+      <c r="B51" s="101" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="116"/>
+      <c r="D51" s="116"/>
+      <c r="E51" s="93"/>
+      <c r="F51" s="86"/>
+    </row>
+    <row r="52" spans="1:6" ht="24" customHeight="1">
+      <c r="A52" s="93"/>
+      <c r="B52" s="101" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" s="116"/>
+      <c r="D52" s="116"/>
+      <c r="E52" s="93"/>
+      <c r="F52" s="86"/>
+    </row>
+    <row r="53" spans="1:6" s="143" customFormat="1" ht="19.2" customHeight="1">
+      <c r="A53" s="145"/>
+      <c r="B53" s="101"/>
+      <c r="C53" s="146"/>
+      <c r="D53" s="146"/>
+      <c r="E53" s="145"/>
+      <c r="F53" s="144"/>
+    </row>
+    <row r="54" spans="1:6" s="87" customFormat="1" ht="26.4" customHeight="1">
+      <c r="A54" s="111"/>
+      <c r="B54" s="110" t="s">
+        <v>152</v>
+      </c>
+      <c r="C54" s="119" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" s="119" t="s">
+        <v>111</v>
+      </c>
+      <c r="E54" s="107" t="s">
+        <v>108</v>
+      </c>
+      <c r="F54" s="86"/>
+    </row>
+    <row r="55" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="A55" s="93"/>
+      <c r="B55" s="101"/>
+      <c r="C55" s="116"/>
+      <c r="D55" s="116"/>
+      <c r="E55" s="93"/>
+      <c r="F55" s="86"/>
+    </row>
+    <row r="56" spans="1:6" s="88" customFormat="1" ht="27.6" customHeight="1">
+      <c r="A56" s="93"/>
+      <c r="B56" s="101" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="116"/>
+      <c r="D56" s="116"/>
+      <c r="E56" s="93"/>
+      <c r="F56" s="86"/>
+    </row>
+    <row r="57" spans="1:6" ht="25.2" customHeight="1">
+      <c r="A57" s="93"/>
+      <c r="B57" s="101" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="116"/>
+      <c r="D57" s="116"/>
+      <c r="E57" s="93"/>
+      <c r="F57" s="86"/>
+    </row>
+    <row r="58" spans="1:6" ht="24.6" customHeight="1">
+      <c r="A58" s="93"/>
+      <c r="B58" s="101" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" s="116"/>
+      <c r="D58" s="116"/>
+      <c r="E58" s="93"/>
+      <c r="F58" s="86"/>
+    </row>
+    <row r="59" spans="1:6" ht="24" customHeight="1">
+      <c r="A59" s="93"/>
+      <c r="B59" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="104"/>
-      <c r="D31" s="104"/>
-      <c r="E31" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="88"/>
-    </row>
-    <row r="32" spans="1:11" ht="15.6">
-      <c r="B32" s="93"/>
-      <c r="F32" s="88"/>
-    </row>
-    <row r="33" spans="1:34" ht="15.6">
-      <c r="B33" s="93" t="s">
+      <c r="C59" s="116"/>
+      <c r="D59" s="116"/>
+      <c r="E59" s="93"/>
+      <c r="F59" s="86"/>
+    </row>
+    <row r="60" spans="1:6" ht="26.4" customHeight="1">
+      <c r="A60" s="93"/>
+      <c r="B60" s="101" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="116"/>
+      <c r="D60" s="116"/>
+      <c r="E60" s="93"/>
+      <c r="F60" s="86"/>
+    </row>
+    <row r="61" spans="1:6" ht="24.6" customHeight="1">
+      <c r="A61" s="93"/>
+      <c r="B61" s="101" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="116"/>
+      <c r="D61" s="116"/>
+      <c r="E61" s="93"/>
+      <c r="F61" s="86"/>
+    </row>
+    <row r="62" spans="1:6" s="89" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A62" s="93"/>
+      <c r="B62" s="101"/>
+      <c r="C62" s="116"/>
+      <c r="D62" s="116"/>
+      <c r="E62" s="93"/>
+      <c r="F62" s="90"/>
+    </row>
+    <row r="63" spans="1:6" s="143" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A63" s="145"/>
+      <c r="B63" s="129" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="119" t="s">
+        <v>155</v>
+      </c>
+      <c r="D63" s="119">
+        <v>43957</v>
+      </c>
+      <c r="E63" s="107" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" s="144"/>
+    </row>
+    <row r="64" spans="1:6" s="143" customFormat="1" ht="31.8" customHeight="1">
+      <c r="A64" s="145"/>
+      <c r="B64" s="112" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="146"/>
+      <c r="D64" s="146"/>
+      <c r="E64" s="145"/>
+      <c r="F64" s="144"/>
+    </row>
+    <row r="65" spans="1:6" s="143" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A65" s="145"/>
+      <c r="B65" s="112" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" s="146"/>
+      <c r="D65" s="146"/>
+      <c r="E65" s="145"/>
+      <c r="F65" s="144"/>
+    </row>
+    <row r="66" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B66" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="C66" s="121"/>
+      <c r="D66" s="121"/>
+    </row>
+    <row r="67" spans="1:6" s="143" customFormat="1" ht="25.8" customHeight="1">
+      <c r="B67" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" s="121"/>
+      <c r="D67" s="121"/>
+    </row>
+    <row r="68" spans="1:6" s="143" customFormat="1" ht="23.4" customHeight="1">
+      <c r="B68" s="112" t="s">
+        <v>104</v>
+      </c>
+      <c r="C68" s="121"/>
+      <c r="D68" s="121"/>
+    </row>
+    <row r="69" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B69" s="112" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" s="121"/>
+      <c r="D69" s="121"/>
+    </row>
+    <row r="70" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B70" s="112" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" s="121"/>
+      <c r="D70" s="121"/>
+    </row>
+    <row r="71" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B71" s="112"/>
+      <c r="C71" s="121"/>
+      <c r="D71" s="121"/>
+    </row>
+    <row r="72" spans="1:6" s="143" customFormat="1" ht="27.6" customHeight="1">
+      <c r="A72" s="145"/>
+      <c r="B72" s="129" t="s">
+        <v>157</v>
+      </c>
+      <c r="C72" s="119">
+        <v>44049</v>
+      </c>
+      <c r="D72" s="119">
+        <v>44171</v>
+      </c>
+      <c r="E72" s="107" t="s">
+        <v>108</v>
+      </c>
+      <c r="F72" s="144"/>
+    </row>
+    <row r="73" spans="1:6" s="143" customFormat="1" ht="14.4" customHeight="1">
+      <c r="A73" s="145"/>
+      <c r="B73" s="127"/>
+      <c r="C73" s="120"/>
+      <c r="D73" s="120"/>
+      <c r="E73" s="144"/>
+      <c r="F73" s="144"/>
+    </row>
+    <row r="74" spans="1:6" s="143" customFormat="1" ht="24" customHeight="1">
+      <c r="A74" s="145"/>
+      <c r="B74" s="112" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" s="120"/>
+      <c r="D74" s="120"/>
+      <c r="E74" s="144"/>
+      <c r="F74" s="144"/>
+    </row>
+    <row r="75" spans="1:6" s="143" customFormat="1" ht="23.4" customHeight="1">
+      <c r="A75" s="145"/>
+      <c r="B75" s="101" t="s">
+        <v>160</v>
+      </c>
+      <c r="C75" s="120"/>
+      <c r="D75" s="120"/>
+      <c r="E75" s="144"/>
+      <c r="F75" s="144"/>
+    </row>
+    <row r="76" spans="1:6" s="143" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A76" s="145"/>
+      <c r="B76" s="112" t="s">
+        <v>163</v>
+      </c>
+      <c r="C76" s="120"/>
+      <c r="D76" s="120"/>
+      <c r="E76" s="144"/>
+      <c r="F76" s="144"/>
+    </row>
+    <row r="77" spans="1:6" s="143" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A77" s="145"/>
+      <c r="B77" s="112" t="s">
+        <v>162</v>
+      </c>
+      <c r="C77" s="120"/>
+      <c r="D77" s="120"/>
+      <c r="E77" s="144"/>
+      <c r="F77" s="144"/>
+    </row>
+    <row r="78" spans="1:6" s="135" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A78" s="131"/>
+      <c r="B78" s="132" t="s">
+        <v>161</v>
+      </c>
+      <c r="C78" s="133"/>
+      <c r="D78" s="133"/>
+      <c r="E78" s="134"/>
+      <c r="F78" s="134"/>
+    </row>
+    <row r="79" spans="1:6" s="135" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A79" s="131"/>
+      <c r="B79" s="132" t="s">
+        <v>159</v>
+      </c>
+      <c r="C79" s="133"/>
+      <c r="D79" s="133"/>
+      <c r="E79" s="134"/>
+      <c r="F79" s="134"/>
+    </row>
+    <row r="80" spans="1:6" s="143" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B80" s="144"/>
+      <c r="C80" s="144"/>
+      <c r="D80" s="144"/>
+      <c r="E80" s="144"/>
+    </row>
+    <row r="81" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B81" s="129" t="s">
+        <v>114</v>
+      </c>
+      <c r="C81" s="130" t="s">
+        <v>115</v>
+      </c>
+      <c r="D81" s="130" t="s">
+        <v>116</v>
+      </c>
+      <c r="E81" s="107" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="144" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B82" s="112" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="144" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B83" s="112" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B84" s="129" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84" s="130" t="s">
+        <v>120</v>
+      </c>
+      <c r="D84" s="130" t="s">
+        <v>121</v>
+      </c>
+      <c r="E84" s="107" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B85" s="113" t="s">
+        <v>118</v>
+      </c>
+      <c r="C85" s="144"/>
+      <c r="D85" s="144"/>
+      <c r="E85" s="144"/>
+    </row>
+    <row r="86" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B86" s="113" t="s">
+        <v>119</v>
+      </c>
+      <c r="C86" s="144"/>
+      <c r="D86" s="144"/>
+      <c r="E86" s="144"/>
+    </row>
+    <row r="87" spans="1:6" s="143" customFormat="1" ht="15.75" customHeight="1">
+      <c r="C87" s="121"/>
+      <c r="D87" s="121"/>
+    </row>
+    <row r="88" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B88" s="90"/>
+      <c r="C88" s="90"/>
+      <c r="D88" s="90"/>
+      <c r="E88" s="90"/>
+    </row>
+    <row r="89" spans="1:6" s="140" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B89" s="144"/>
+      <c r="C89" s="144"/>
+      <c r="D89" s="144"/>
+      <c r="E89" s="144"/>
+    </row>
+    <row r="90" spans="1:6" s="142" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B90" s="144"/>
+      <c r="C90" s="144"/>
+      <c r="D90" s="144"/>
+      <c r="E90" s="144"/>
+    </row>
+    <row r="91" spans="1:6" s="142" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B91" s="144"/>
+      <c r="C91" s="144"/>
+      <c r="D91" s="144"/>
+      <c r="E91" s="144"/>
+    </row>
+    <row r="92" spans="1:6" s="140" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B92" s="144"/>
+      <c r="C92" s="144"/>
+      <c r="D92" s="144"/>
+      <c r="E92" s="144"/>
+    </row>
+    <row r="93" spans="1:6" s="140" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B93" s="113"/>
+      <c r="C93" s="144"/>
+      <c r="D93" s="144"/>
+      <c r="E93" s="144"/>
+    </row>
+    <row r="94" spans="1:6" s="140" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B94" s="113"/>
+      <c r="C94" s="144"/>
+      <c r="D94" s="144"/>
+      <c r="E94" s="144"/>
+    </row>
+    <row r="95" spans="1:6" s="140" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A95" s="141"/>
+      <c r="B95" s="112"/>
+      <c r="C95" s="144"/>
+      <c r="D95" s="144"/>
+      <c r="E95" s="144"/>
+      <c r="F95" s="142"/>
+    </row>
+    <row r="96" spans="1:6" s="140" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A96" s="141"/>
+      <c r="B96" s="112"/>
+      <c r="C96" s="120"/>
+      <c r="D96" s="120"/>
+      <c r="E96" s="142"/>
+      <c r="F96" s="142"/>
+    </row>
+    <row r="97" spans="1:6" s="135" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A97" s="131"/>
+      <c r="B97" s="132"/>
+      <c r="C97" s="133"/>
+      <c r="D97" s="133"/>
+      <c r="E97" s="134"/>
+      <c r="F97" s="134"/>
+    </row>
+    <row r="98" spans="1:6" s="135" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A98" s="131"/>
+      <c r="B98" s="132"/>
+      <c r="C98" s="133"/>
+      <c r="D98" s="133"/>
+      <c r="E98" s="134"/>
+      <c r="F98" s="134"/>
+    </row>
+    <row r="99" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B99" s="89"/>
+    </row>
+    <row r="100" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B100" s="89"/>
+    </row>
+    <row r="101" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B101" s="89"/>
+    </row>
+    <row r="102" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B102" s="89"/>
+    </row>
+    <row r="103" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B103" s="89"/>
+    </row>
+    <row r="104" spans="1:6" s="143" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A104" s="145"/>
+      <c r="B104" s="129" t="s">
+        <v>147</v>
+      </c>
+      <c r="C104" s="119">
+        <v>43836</v>
+      </c>
+      <c r="D104" s="119">
+        <v>44171</v>
+      </c>
+      <c r="E104" s="107" t="s">
+        <v>89</v>
+      </c>
+      <c r="F104" s="144"/>
+    </row>
+    <row r="105" spans="1:6" s="143" customFormat="1" ht="31.8" customHeight="1">
+      <c r="A105" s="145"/>
+      <c r="B105" s="112" t="s">
+        <v>106</v>
+      </c>
+      <c r="C105" s="146"/>
+      <c r="D105" s="146"/>
+      <c r="E105" s="145"/>
+      <c r="F105" s="144"/>
+    </row>
+    <row r="106" spans="1:6" s="143" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A106" s="145"/>
+      <c r="B106" s="112" t="s">
+        <v>151</v>
+      </c>
+      <c r="C106" s="146"/>
+      <c r="D106" s="146"/>
+      <c r="E106" s="145"/>
+      <c r="F106" s="144"/>
+    </row>
+    <row r="107" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B107" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="C107" s="121"/>
+      <c r="D107" s="121"/>
+    </row>
+    <row r="108" spans="1:6" s="143" customFormat="1" ht="25.8" customHeight="1">
+      <c r="B108" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="C108" s="121"/>
+      <c r="D108" s="121"/>
+    </row>
+    <row r="109" spans="1:6" s="143" customFormat="1" ht="23.4" customHeight="1">
+      <c r="B109" s="112" t="s">
+        <v>104</v>
+      </c>
+      <c r="C109" s="121"/>
+      <c r="D109" s="121"/>
+    </row>
+    <row r="110" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B110" s="112" t="s">
+        <v>98</v>
+      </c>
+      <c r="C110" s="121"/>
+      <c r="D110" s="121"/>
+    </row>
+    <row r="111" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B111" s="112" t="s">
+        <v>105</v>
+      </c>
+      <c r="C111" s="121"/>
+      <c r="D111" s="121"/>
+    </row>
+    <row r="112" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B112" s="112"/>
+      <c r="C112" s="121"/>
+      <c r="D112" s="121"/>
+    </row>
+    <row r="113" spans="1:6" s="143" customFormat="1" ht="27.6" customHeight="1">
+      <c r="A113" s="145"/>
+      <c r="B113" s="129" t="s">
+        <v>148</v>
+      </c>
+      <c r="C113" s="119" t="s">
         <v>112</v>
       </c>
-      <c r="F33" s="88"/>
-    </row>
-    <row r="34" spans="1:34" ht="15.6">
-      <c r="B34" s="93" t="s">
+      <c r="D113" s="119" t="s">
         <v>113</v>
       </c>
-      <c r="F34" s="88"/>
-    </row>
-    <row r="35" spans="1:34" ht="15.6">
-      <c r="B35" s="93" t="s">
-        <v>83</v>
-      </c>
-      <c r="F35" s="88"/>
-    </row>
-    <row r="36" spans="1:34" ht="15" customHeight="1">
-      <c r="B36" s="93" t="s">
-        <v>93</v>
-      </c>
-      <c r="F36" s="88"/>
-    </row>
-    <row r="37" spans="1:34" s="85" customFormat="1" ht="19.8" customHeight="1">
-      <c r="A37" s="109"/>
-      <c r="B37" s="96" t="s">
-        <v>95</v>
-      </c>
-      <c r="E37" s="107" t="s">
-        <v>100</v>
-      </c>
-      <c r="F37" s="88"/>
-      <c r="G37" s="88"/>
-      <c r="H37" s="88"/>
-      <c r="I37" s="88"/>
-      <c r="J37" s="88"/>
-      <c r="K37" s="88"/>
-      <c r="L37" s="88"/>
-      <c r="M37" s="88"/>
-      <c r="N37" s="88"/>
-      <c r="O37" s="88"/>
-      <c r="P37" s="88"/>
-      <c r="Q37" s="88"/>
-      <c r="R37" s="88"/>
-      <c r="S37" s="88"/>
-      <c r="T37" s="88"/>
-      <c r="U37" s="88"/>
-      <c r="V37" s="88"/>
-      <c r="W37" s="88"/>
-      <c r="X37" s="88"/>
-      <c r="Y37" s="88"/>
-      <c r="Z37" s="88"/>
-      <c r="AA37" s="88"/>
-      <c r="AB37" s="88"/>
-      <c r="AC37" s="88"/>
-      <c r="AD37" s="88"/>
-      <c r="AE37" s="88"/>
-      <c r="AF37" s="88"/>
-      <c r="AG37" s="88"/>
-      <c r="AH37" s="88"/>
-    </row>
-    <row r="38" spans="1:34" ht="15.6">
-      <c r="B38" s="93"/>
-      <c r="F38" s="88"/>
-    </row>
-    <row r="39" spans="1:34" ht="15.6">
-      <c r="B39" s="93" t="s">
-        <v>106</v>
-      </c>
-      <c r="F39" s="88"/>
-    </row>
-    <row r="40" spans="1:34" ht="16.8" customHeight="1">
-      <c r="B40" s="93" t="s">
-        <v>107</v>
-      </c>
-      <c r="F40" s="88"/>
-    </row>
-    <row r="41" spans="1:34" ht="15.6" customHeight="1">
-      <c r="B41" s="93" t="s">
-        <v>85</v>
-      </c>
-      <c r="F41" s="88"/>
-    </row>
-    <row r="42" spans="1:34" s="84" customFormat="1" ht="15.6" customHeight="1">
-      <c r="B42" s="93" t="s">
-        <v>94</v>
-      </c>
-      <c r="F42" s="88"/>
-    </row>
-    <row r="43" spans="1:34" ht="15" customHeight="1">
-      <c r="B43" s="93" t="s">
-        <v>93</v>
-      </c>
-      <c r="F43" s="88"/>
-    </row>
-    <row r="44" spans="1:34" ht="13.2" customHeight="1">
-      <c r="B44" s="93" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" s="88"/>
-    </row>
-    <row r="45" spans="1:34" s="89" customFormat="1" ht="21" customHeight="1">
-      <c r="B45" s="96" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="85"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="107" t="s">
-        <v>100</v>
-      </c>
-      <c r="F45" s="88"/>
-    </row>
-    <row r="46" spans="1:34" ht="14.4" customHeight="1">
-      <c r="B46" s="93"/>
-      <c r="F46" s="88"/>
-    </row>
-    <row r="47" spans="1:34" s="105" customFormat="1" ht="15.6" customHeight="1">
-      <c r="B47" s="93" t="s">
+      <c r="E113" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="F47" s="88"/>
-    </row>
-    <row r="48" spans="1:34" ht="15.75" customHeight="1">
-      <c r="B48" s="93" t="s">
+      <c r="F113" s="144"/>
+    </row>
+    <row r="114" spans="1:6" s="143" customFormat="1" ht="14.4" customHeight="1">
+      <c r="A114" s="145"/>
+      <c r="B114" s="127"/>
+      <c r="C114" s="120"/>
+      <c r="D114" s="120"/>
+      <c r="E114" s="144"/>
+      <c r="F114" s="144"/>
+    </row>
+    <row r="115" spans="1:6" s="143" customFormat="1" ht="24" customHeight="1">
+      <c r="A115" s="145"/>
+      <c r="B115" s="112" t="s">
+        <v>136</v>
+      </c>
+      <c r="C115" s="120"/>
+      <c r="D115" s="120"/>
+      <c r="E115" s="144"/>
+      <c r="F115" s="144"/>
+    </row>
+    <row r="116" spans="1:6" s="143" customFormat="1" ht="23.4" customHeight="1">
+      <c r="A116" s="145"/>
+      <c r="B116" s="101" t="s">
+        <v>137</v>
+      </c>
+      <c r="C116" s="120"/>
+      <c r="D116" s="120"/>
+      <c r="E116" s="144"/>
+      <c r="F116" s="144"/>
+    </row>
+    <row r="117" spans="1:6" s="143" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A117" s="145"/>
+      <c r="B117" s="112" t="s">
         <v>101</v>
       </c>
-      <c r="F48" s="88"/>
-    </row>
-    <row r="49" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B49" s="93" t="s">
-        <v>87</v>
-      </c>
-      <c r="F49" s="88"/>
-    </row>
-    <row r="50" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B50" s="93" t="s">
-        <v>97</v>
-      </c>
-      <c r="F50" s="88"/>
-    </row>
-    <row r="51" spans="2:6" s="84" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B51" s="93" t="s">
-        <v>98</v>
-      </c>
-      <c r="F51" s="88"/>
-    </row>
-    <row r="52" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B52" s="93" t="s">
-        <v>88</v>
-      </c>
-      <c r="F52" s="88"/>
-    </row>
-    <row r="53" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B53" s="93" t="s">
-        <v>89</v>
-      </c>
-      <c r="F53" s="88"/>
-    </row>
-    <row r="54" spans="2:6" ht="20.399999999999999" customHeight="1">
-      <c r="B54" s="131" t="s">
+      <c r="C117" s="120"/>
+      <c r="D117" s="120"/>
+      <c r="E117" s="144"/>
+      <c r="F117" s="144"/>
+    </row>
+    <row r="118" spans="1:6" s="143" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A118" s="145"/>
+      <c r="B118" s="112" t="s">
+        <v>102</v>
+      </c>
+      <c r="C118" s="120"/>
+      <c r="D118" s="120"/>
+      <c r="E118" s="144"/>
+      <c r="F118" s="144"/>
+    </row>
+    <row r="119" spans="1:6" s="135" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A119" s="131"/>
+      <c r="B119" s="132" t="s">
+        <v>153</v>
+      </c>
+      <c r="C119" s="133"/>
+      <c r="D119" s="133"/>
+      <c r="E119" s="134"/>
+      <c r="F119" s="134"/>
+    </row>
+    <row r="120" spans="1:6" s="135" customFormat="1" ht="25.8" customHeight="1">
+      <c r="A120" s="131"/>
+      <c r="B120" s="132" t="s">
+        <v>138</v>
+      </c>
+      <c r="C120" s="133"/>
+      <c r="D120" s="133"/>
+      <c r="E120" s="134"/>
+      <c r="F120" s="134"/>
+    </row>
+    <row r="121" spans="1:6" s="143" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B121" s="144"/>
+      <c r="C121" s="144"/>
+      <c r="D121" s="144"/>
+      <c r="E121" s="144"/>
+    </row>
+    <row r="122" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B122" s="129" t="s">
+        <v>114</v>
+      </c>
+      <c r="C122" s="130" t="s">
+        <v>115</v>
+      </c>
+      <c r="D122" s="130" t="s">
+        <v>116</v>
+      </c>
+      <c r="E122" s="107" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" s="144" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B123" s="112" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" s="144" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B124" s="112" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B125" s="129" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="85"/>
-      <c r="D54" s="85"/>
-      <c r="E54" s="108" t="s">
-        <v>73</v>
-      </c>
-      <c r="F54" s="88"/>
-    </row>
-    <row r="55" spans="2:6" ht="21" customHeight="1">
-      <c r="B55" s="131" t="s">
+      <c r="C125" s="130" t="s">
+        <v>120</v>
+      </c>
+      <c r="D125" s="130" t="s">
+        <v>121</v>
+      </c>
+      <c r="E125" s="107" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B126" s="113" t="s">
         <v>118</v>
       </c>
-      <c r="C55" s="85"/>
-      <c r="D55" s="85"/>
-      <c r="E55" s="130" t="s">
-        <v>100</v>
-      </c>
-      <c r="F55" s="88"/>
-    </row>
-    <row r="56" spans="2:6" ht="15.75" customHeight="1">
-      <c r="F56" s="88"/>
-    </row>
-    <row r="57" spans="2:6" ht="15.75" customHeight="1">
-      <c r="F57" s="88"/>
+      <c r="C126" s="144"/>
+      <c r="D126" s="144"/>
+      <c r="E126" s="144"/>
+    </row>
+    <row r="127" spans="1:6" s="143" customFormat="1" ht="25.2" customHeight="1">
+      <c r="B127" s="113" t="s">
+        <v>119</v>
+      </c>
+      <c r="C127" s="144"/>
+      <c r="D127" s="144"/>
+      <c r="E127" s="144"/>
+    </row>
+    <row r="128" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B128" s="89"/>
+    </row>
+    <row r="129" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B129" s="89"/>
+    </row>
+    <row r="130" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B130" s="89"/>
+    </row>
+    <row r="131" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B131" s="89"/>
+    </row>
+    <row r="132" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B132" s="89"/>
+    </row>
+    <row r="133" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B133" s="89"/>
+    </row>
+    <row r="134" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B134" s="89"/>
+    </row>
+    <row r="135" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B135" s="89"/>
+    </row>
+    <row r="136" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B136" s="89"/>
+    </row>
+    <row r="137" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B137" s="89"/>
+    </row>
+    <row r="138" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B138" s="89"/>
+    </row>
+    <row r="139" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B139" s="89"/>
+    </row>
+    <row r="140" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B140" s="89"/>
+    </row>
+    <row r="141" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B141" s="89"/>
+    </row>
+    <row r="142" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B142" s="89"/>
+    </row>
+    <row r="143" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B143" s="89"/>
+    </row>
+    <row r="144" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B144" s="89"/>
+    </row>
+    <row r="145" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B145" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4153,7 +5170,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25">
+  <conditionalFormatting sqref="F28">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="percent" val="0"/>
@@ -4163,7 +5180,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F17 F11:F12 F21:F24">
+  <conditionalFormatting sqref="F16:F19 F11:F13 F24:F27">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="percent" val="0"/>
@@ -4174,7 +5191,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="D15:D17 C9:D12 D21:D25" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="D16:D19 C9:D13 D24:D28" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(C9))), AND(ISNUMBER(C9), LEFT(CELL("format", C9))="D"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -4342,15 +5359,15 @@
       <c r="BO2" s="2"/>
     </row>
     <row r="3" spans="1:67" ht="30" customHeight="1">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
+      <c r="B3" s="155"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="155"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -4551,118 +5568,118 @@
       <c r="BO5" s="2"/>
     </row>
     <row r="6" spans="1:67" ht="14.4">
-      <c r="A6" s="110"/>
-      <c r="B6" s="110" t="s">
+      <c r="A6" s="147"/>
+      <c r="B6" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="147" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="110" t="s">
+      <c r="D6" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="110" t="s">
+      <c r="E6" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="110" t="s">
+      <c r="F6" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="124" t="s">
+      <c r="G6" s="164" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="126" t="s">
+      <c r="H6" s="166" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="122"/>
-      <c r="J6" s="122"/>
-      <c r="K6" s="122"/>
-      <c r="L6" s="122"/>
-      <c r="M6" s="121" t="s">
+      <c r="I6" s="162"/>
+      <c r="J6" s="162"/>
+      <c r="K6" s="162"/>
+      <c r="L6" s="162"/>
+      <c r="M6" s="161" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="122"/>
-      <c r="O6" s="122"/>
-      <c r="P6" s="122"/>
-      <c r="Q6" s="122"/>
-      <c r="R6" s="126" t="s">
+      <c r="N6" s="162"/>
+      <c r="O6" s="162"/>
+      <c r="P6" s="162"/>
+      <c r="Q6" s="162"/>
+      <c r="R6" s="166" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="122"/>
-      <c r="T6" s="122"/>
-      <c r="U6" s="122"/>
-      <c r="V6" s="122"/>
-      <c r="W6" s="121" t="s">
+      <c r="S6" s="162"/>
+      <c r="T6" s="162"/>
+      <c r="U6" s="162"/>
+      <c r="V6" s="162"/>
+      <c r="W6" s="161" t="s">
         <v>10</v>
       </c>
-      <c r="X6" s="122"/>
-      <c r="Y6" s="122"/>
-      <c r="Z6" s="122"/>
-      <c r="AA6" s="122"/>
-      <c r="AB6" s="126" t="s">
+      <c r="X6" s="162"/>
+      <c r="Y6" s="162"/>
+      <c r="Z6" s="162"/>
+      <c r="AA6" s="162"/>
+      <c r="AB6" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="AC6" s="122"/>
-      <c r="AD6" s="122"/>
-      <c r="AE6" s="122"/>
-      <c r="AF6" s="122"/>
-      <c r="AG6" s="121" t="s">
+      <c r="AC6" s="162"/>
+      <c r="AD6" s="162"/>
+      <c r="AE6" s="162"/>
+      <c r="AF6" s="162"/>
+      <c r="AG6" s="161" t="s">
         <v>12</v>
       </c>
-      <c r="AH6" s="122"/>
-      <c r="AI6" s="122"/>
-      <c r="AJ6" s="122"/>
-      <c r="AK6" s="122"/>
-      <c r="AL6" s="126" t="s">
+      <c r="AH6" s="162"/>
+      <c r="AI6" s="162"/>
+      <c r="AJ6" s="162"/>
+      <c r="AK6" s="162"/>
+      <c r="AL6" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="AM6" s="122"/>
-      <c r="AN6" s="122"/>
-      <c r="AO6" s="122"/>
-      <c r="AP6" s="122"/>
-      <c r="AQ6" s="121" t="s">
+      <c r="AM6" s="162"/>
+      <c r="AN6" s="162"/>
+      <c r="AO6" s="162"/>
+      <c r="AP6" s="162"/>
+      <c r="AQ6" s="161" t="s">
         <v>14</v>
       </c>
-      <c r="AR6" s="122"/>
-      <c r="AS6" s="122"/>
-      <c r="AT6" s="122"/>
-      <c r="AU6" s="122"/>
-      <c r="AV6" s="126" t="s">
+      <c r="AR6" s="162"/>
+      <c r="AS6" s="162"/>
+      <c r="AT6" s="162"/>
+      <c r="AU6" s="162"/>
+      <c r="AV6" s="166" t="s">
         <v>15</v>
       </c>
-      <c r="AW6" s="122"/>
-      <c r="AX6" s="122"/>
-      <c r="AY6" s="122"/>
-      <c r="AZ6" s="122"/>
-      <c r="BA6" s="121" t="s">
+      <c r="AW6" s="162"/>
+      <c r="AX6" s="162"/>
+      <c r="AY6" s="162"/>
+      <c r="AZ6" s="162"/>
+      <c r="BA6" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="BB6" s="122"/>
-      <c r="BC6" s="122"/>
-      <c r="BD6" s="122"/>
-      <c r="BE6" s="122"/>
-      <c r="BF6" s="126" t="s">
+      <c r="BB6" s="162"/>
+      <c r="BC6" s="162"/>
+      <c r="BD6" s="162"/>
+      <c r="BE6" s="162"/>
+      <c r="BF6" s="166" t="s">
         <v>17</v>
       </c>
-      <c r="BG6" s="122"/>
-      <c r="BH6" s="122"/>
-      <c r="BI6" s="122"/>
-      <c r="BJ6" s="122"/>
-      <c r="BK6" s="121" t="s">
+      <c r="BG6" s="162"/>
+      <c r="BH6" s="162"/>
+      <c r="BI6" s="162"/>
+      <c r="BJ6" s="162"/>
+      <c r="BK6" s="161" t="s">
         <v>18</v>
       </c>
-      <c r="BL6" s="122"/>
-      <c r="BM6" s="122"/>
-      <c r="BN6" s="122"/>
-      <c r="BO6" s="122"/>
+      <c r="BL6" s="162"/>
+      <c r="BM6" s="162"/>
+      <c r="BN6" s="162"/>
+      <c r="BO6" s="162"/>
     </row>
     <row r="7" spans="1:67" ht="14.4">
-      <c r="A7" s="111"/>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="125"/>
+      <c r="A7" s="148"/>
+      <c r="B7" s="148"/>
+      <c r="C7" s="148"/>
+      <c r="D7" s="148"/>
+      <c r="E7" s="148"/>
+      <c r="F7" s="148"/>
+      <c r="G7" s="165"/>
       <c r="H7" s="10" t="s">
         <v>19</v>
       </c>
@@ -4849,11 +5866,11 @@
         <v>24</v>
       </c>
       <c r="B8" s="15"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="128"/>
-      <c r="E8" s="128"/>
-      <c r="F8" s="128"/>
-      <c r="G8" s="128"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="168"/>
+      <c r="E8" s="168"/>
+      <c r="F8" s="168"/>
+      <c r="G8" s="168"/>
       <c r="H8" s="16"/>
       <c r="I8" s="17"/>
       <c r="J8" s="18"/>
@@ -5400,11 +6417,11 @@
         <v>36</v>
       </c>
       <c r="B15" s="35"/>
-      <c r="C15" s="127"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
-      <c r="F15" s="128"/>
-      <c r="G15" s="128"/>
+      <c r="C15" s="167"/>
+      <c r="D15" s="168"/>
+      <c r="E15" s="168"/>
+      <c r="F15" s="168"/>
+      <c r="G15" s="168"/>
       <c r="H15" s="36"/>
       <c r="I15" s="37"/>
       <c r="J15" s="38"/>
@@ -5795,11 +6812,11 @@
         <v>41</v>
       </c>
       <c r="B20" s="35"/>
-      <c r="C20" s="127"/>
-      <c r="D20" s="128"/>
-      <c r="E20" s="128"/>
-      <c r="F20" s="128"/>
-      <c r="G20" s="128"/>
+      <c r="C20" s="167"/>
+      <c r="D20" s="168"/>
+      <c r="E20" s="168"/>
+      <c r="F20" s="168"/>
+      <c r="G20" s="168"/>
       <c r="H20" s="36"/>
       <c r="I20" s="37"/>
       <c r="J20" s="38"/>
@@ -6352,11 +7369,11 @@
         <v>48</v>
       </c>
       <c r="B27" s="35"/>
-      <c r="C27" s="127"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="128"/>
-      <c r="F27" s="128"/>
-      <c r="G27" s="128"/>
+      <c r="C27" s="167"/>
+      <c r="D27" s="168"/>
+      <c r="E27" s="168"/>
+      <c r="F27" s="168"/>
+      <c r="G27" s="168"/>
       <c r="H27" s="36"/>
       <c r="I27" s="37"/>
       <c r="J27" s="38"/>

</xml_diff>